<commit_message>
added CLI, changed casing to be schematic compliant
</commit_message>
<xml_diff>
--- a/project/excel/include_schema.xlsx
+++ b/project/excel/include_schema.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="17" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Aliquot" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Biospecimen" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Condition" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataFile" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FamilyGroup" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Participant" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Study" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thing" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Aliquot1" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay1" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Biospecimen1" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Condition1" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataFile1" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FamilyGroup1" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Participant1" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Study1" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thing1" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet name="Aliquot" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Assay" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Biospecimen" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Condition" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="DataFile" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="FamilyGroup" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Participant" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Study" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Thing" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Aliquot1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Assay1" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Biospecimen1" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Condition1" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="DataFile1" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="FamilyGroup1" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Participant1" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="Study1" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet name="Thing1" sheetId="18" state="visible" r:id="rId18"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -477,12 +477,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>uses_biospecimen</t>
+          <t>UsesBiospecimen</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>has_output</t>
+          <t>HasOutput</t>
         </is>
       </c>
     </row>
@@ -508,87 +508,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>age_at_biospecimen_collection</t>
+          <t>AgeAtBiospecimenCollection</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biospecimen_storage</t>
+          <t>BiospecimenStorage</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>collection_id</t>
+          <t>CollectionID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>collection_sample_type</t>
+          <t>CollectionSampleType</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>container_id</t>
+          <t>ContainerID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>has_datafile</t>
+          <t>HasDatafile</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>has_study</t>
+          <t>HasStudy</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>laboratory_procedure</t>
+          <t>LaboratoryProcedure</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>parent_sample_id</t>
+          <t>ParentSampleID</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>parent_sample_type</t>
+          <t>ParentSampleType</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>sample_availability</t>
+          <t>SampleAvailability</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>sample_id</t>
+          <t>SampleID</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>sample_type</t>
+          <t>SampleType</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>volume</t>
+          <t>Volume</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>volume_unit</t>
+          <t>VolumeUnit</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>has_aliquot</t>
+          <t>HasAliquot</t>
         </is>
       </c>
     </row>
@@ -614,62 +614,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>age_at_condition_observation</t>
+          <t>AgeAtConditionObservation</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>mondo_label</t>
+          <t>MONDOLabel</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>mondo_code</t>
+          <t>MONDOCode</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>condition_interpretation</t>
+          <t>ConditionInterpretation</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>condition_data_source</t>
+          <t>ConditionDataSource</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>hpo_label</t>
+          <t>HPOLabel</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>hpo_code</t>
+          <t>HPOCode</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>maxo_label</t>
+          <t>MAXOLabel</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>maxo_code</t>
+          <t>MAXOCode</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>other_label</t>
+          <t>OtherLabel</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>other_code</t>
+          <t>OtherCode</t>
         </is>
       </c>
     </row>
@@ -695,77 +695,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>access_url</t>
+          <t>AccessURL</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>collection_id</t>
+          <t>CollectionID</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>data_access</t>
+          <t>DataAccess</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>data_category</t>
+          <t>DataCategory</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>data_type</t>
+          <t>DataType</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>experimental_strategy</t>
+          <t>ExperimentalStrategy</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>file_id</t>
+          <t>FileID</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>file_name</t>
+          <t>FileName</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>format</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>has_biospecimen</t>
+          <t>HasBiospecimen</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>has_study</t>
+          <t>HasStudy</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>participant_id</t>
+          <t>ParticipantID</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>size</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>original_file_name</t>
+          <t>OriginalFileName</t>
         </is>
       </c>
     </row>
@@ -791,7 +791,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
     </row>
@@ -817,77 +817,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>age_at_last_vital_status</t>
+          <t>AgeAtLastVitalStatus</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>down_syndrome_status</t>
+          <t>DownSyndromeStatus</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ethnicity</t>
+          <t>Ethnicity</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>external_id</t>
+          <t>ExternalID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>family_id</t>
+          <t>FamilyID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>family_relationship</t>
+          <t>FamilyRelationship</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>family_type</t>
+          <t>FamilyType</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>father_id</t>
+          <t>FatherID</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>has_datafile</t>
+          <t>HasDatafile</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>has_study</t>
+          <t>HasStudy</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>mother_id</t>
+          <t>MotherID</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>outcomes_vital_status</t>
+          <t>OutcomesVitalStatus</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>participant_id</t>
+          <t>ParticipantID</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>race</t>
+          <t>Race</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>Sex</t>
         </is>
       </c>
     </row>
@@ -902,7 +902,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,22 +913,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>dbgap</t>
+          <t>dbGap</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>program</t>
+          <t>Program</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>study_code</t>
+          <t>StudyCode</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>study_name</t>
+          <t>StudyName</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>HasParticipant</t>
         </is>
       </c>
     </row>
@@ -972,12 +977,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>uses_biospecimen</t>
+          <t>UsesBiospecimen</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>has_output</t>
+          <t>HasOutput</t>
         </is>
       </c>
     </row>
@@ -1003,87 +1008,87 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>age_at_biospecimen_collection</t>
+          <t>AgeAtBiospecimenCollection</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>biospecimen_storage</t>
+          <t>BiospecimenStorage</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>collection_id</t>
+          <t>CollectionID</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>collection_sample_type</t>
+          <t>CollectionSampleType</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>container_id</t>
+          <t>ContainerID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>has_datafile</t>
+          <t>HasDatafile</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>has_study</t>
+          <t>HasStudy</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>laboratory_procedure</t>
+          <t>LaboratoryProcedure</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>parent_sample_id</t>
+          <t>ParentSampleID</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>parent_sample_type</t>
+          <t>ParentSampleType</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>sample_availability</t>
+          <t>SampleAvailability</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>sample_id</t>
+          <t>SampleID</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>sample_type</t>
+          <t>SampleType</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>volume</t>
+          <t>Volume</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>volume_unit</t>
+          <t>VolumeUnit</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>has_aliquot</t>
+          <t>HasAliquot</t>
         </is>
       </c>
     </row>
@@ -1117,62 +1122,62 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>age_at_condition_observation</t>
+          <t>AgeAtConditionObservation</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>mondo_label</t>
+          <t>MONDOLabel</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>mondo_code</t>
+          <t>MONDOCode</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>condition_interpretation</t>
+          <t>ConditionInterpretation</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>condition_data_source</t>
+          <t>ConditionDataSource</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>hpo_label</t>
+          <t>HPOLabel</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>hpo_code</t>
+          <t>HPOCode</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>maxo_label</t>
+          <t>MAXOLabel</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>maxo_code</t>
+          <t>MAXOCode</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>other_label</t>
+          <t>OtherLabel</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>other_code</t>
+          <t>OtherCode</t>
         </is>
       </c>
     </row>
@@ -1212,77 +1217,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>access_url</t>
+          <t>AccessURL</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>collection_id</t>
+          <t>CollectionID</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>data_access</t>
+          <t>DataAccess</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>data_category</t>
+          <t>DataCategory</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>data_type</t>
+          <t>DataType</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>experimental_strategy</t>
+          <t>ExperimentalStrategy</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>file_id</t>
+          <t>FileID</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>file_name</t>
+          <t>FileName</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>format</t>
+          <t>Format</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>has_biospecimen</t>
+          <t>HasBiospecimen</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>has_study</t>
+          <t>HasStudy</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>participant_id</t>
+          <t>ParticipantID</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>size</t>
+          <t>Size</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>original_file_name</t>
+          <t>OriginalFileName</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1321,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>has_participant</t>
+          <t>HasParticipant</t>
         </is>
       </c>
     </row>
@@ -1342,77 +1347,77 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>age_at_last_vital_status</t>
+          <t>AgeAtLastVitalStatus</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>down_syndrome_status</t>
+          <t>DownSyndromeStatus</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>ethnicity</t>
+          <t>Ethnicity</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>external_id</t>
+          <t>ExternalID</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>family_id</t>
+          <t>FamilyID</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>family_relationship</t>
+          <t>FamilyRelationship</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>family_type</t>
+          <t>FamilyType</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>father_id</t>
+          <t>FatherID</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>has_datafile</t>
+          <t>HasDatafile</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>has_study</t>
+          <t>HasStudy</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>mother_id</t>
+          <t>MotherID</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>outcomes_vital_status</t>
+          <t>OutcomesVitalStatus</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>participant_id</t>
+          <t>ParticipantID</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>race</t>
+          <t>Race</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>sex</t>
+          <t>Sex</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1436,7 @@
       <formula1>"dead,alive"</formula1>
     </dataValidation>
     <dataValidation sqref="N2:N1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"american_indian_or_alaskan_native,asian,black_or_african_american,more_than_one_race,native_hawaiian_or_other_pacific_islander,other,white,prefer_not_to_answer"</formula1>
+      <formula1>"american_indian_or_alaskan_native,asian,black_or_african_american,more_than_one_Race,native_hawaiian_or_other_pacific_islander,other,white,prefer_not_to_answer"</formula1>
     </dataValidation>
     <dataValidation sqref="O2:O1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"female,male,other,unknown"</formula1>
@@ -1449,7 +1454,7 @@
       <formula1>"dead,alive"</formula1>
     </dataValidation>
     <dataValidation sqref="N2:N1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
-      <formula1>"american_indian_or_alaskan_native,asian,black_or_african_american,more_than_one_race,native_hawaiian_or_other_pacific_islander,other,white,prefer_not_to_answer"</formula1>
+      <formula1>"american_indian_or_alaskan_native,asian,black_or_african_american,more_than_one_Race,native_hawaiian_or_other_pacific_islander,other,white,prefer_not_to_answer"</formula1>
     </dataValidation>
     <dataValidation sqref="O2:O1048576" showErrorMessage="1" showInputMessage="1" allowBlank="1" type="list">
       <formula1>"female,male,other,unknown"</formula1>
@@ -1465,7 +1470,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1476,22 +1481,27 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>dbgap</t>
+          <t>dbGap</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>program</t>
+          <t>Program</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>study_code</t>
+          <t>StudyCode</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>study_name</t>
+          <t>StudyName</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>HasParticipant</t>
         </is>
       </c>
     </row>

</xml_diff>